<commit_message>
update ICO for Alaska w/ culturally important mammals and birds
</commit_message>
<xml_diff>
--- a/circle2016/prep/AO/fish/artisinal_fished.xlsx
+++ b/circle2016/prep/AO/fish/artisinal_fished.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MB4514\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MB4514\Documents\github\arc\circle2016\prep\AO\fish\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="134">
   <si>
     <t>sciname</t>
   </si>
@@ -777,13 +780,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119:G137"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -801,10 +807,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -815,164 +821,164 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -983,10 +989,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -997,1721 +1003,1712 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="D51" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C53" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
         <v>8</v>
-      </c>
-      <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C63" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D63" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C68" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D75" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C76" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C77" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D78" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C79" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D79" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="D82" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D83" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D84" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="D86" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D87" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D88" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C89" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D91" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C92" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="D92" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C93" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D93" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C94" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D94" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C95" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C96" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D96" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="D98" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C99" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="D99" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C100" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="D100" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C101" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="D101" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D102" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C103" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="D103" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D104" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D105" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C106" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D106" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C107" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D107" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C108" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="D108" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C109" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="D109" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C110" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D110" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C111" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="D111" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C112" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D112" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="D113" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>94</v>
+      </c>
+      <c r="C114" t="s">
         <v>3</v>
       </c>
-      <c r="B114" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114" t="s">
-        <v>29</v>
-      </c>
       <c r="D114" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C115" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="D115" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C116" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C117" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="D117" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C118" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="D118" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="D119" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C120" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D120" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C121" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="D121" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C122" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D122" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C123" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C124" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="D124" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C125" t="s">
-        <v>124</v>
+        <v>53</v>
       </c>
       <c r="D125" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C126" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="D126" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="D127" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C128" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D128" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="D129" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C130" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="D130" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B131" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C131" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="D131" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B132" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C132" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D132" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B133" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C133" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="D133" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C134" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D134" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C135" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="D135" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B136" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C136" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D136" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C137" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D137" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138">
-        <v>1</v>
-      </c>
-      <c r="B138" t="s">
-        <v>115</v>
-      </c>
-      <c r="C138" t="s">
-        <v>132</v>
-      </c>
-      <c r="D138" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1">
+    <sortState ref="A2:D138">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>